<commit_message>
add sources, fix references in test plans
</commit_message>
<xml_diff>
--- a/project/fractal-parallel-tasks/test-plan-2.xlsx
+++ b/project/fractal-parallel-tasks/test-plan-2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096"/>
   </bookViews>
   <sheets>
     <sheet name="image-size" sheetId="1" r:id="rId1"/>
@@ -1320,11 +1320,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1415006048"/>
-        <c:axId val="1414991904"/>
+        <c:axId val="-77692064"/>
+        <c:axId val="-77691520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1415006048"/>
+        <c:axId val="-77692064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1428,7 +1428,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1414991904"/>
+        <c:crossAx val="-77691520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1436,7 +1436,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1414991904"/>
+        <c:axId val="-77691520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1544,7 +1544,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1415006048"/>
+        <c:crossAx val="-77692064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1725,7 +1725,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'image-size'!$D$7:$D$19</c:f>
+              <c:f>iterations!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1841,7 +1841,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'image-size'!$D$7:$D$19</c:f>
+              <c:f>iterations!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1957,7 +1957,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'image-size'!$D$7:$D$19</c:f>
+              <c:f>iterations!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2073,7 +2073,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'image-size'!$D$7:$D$19</c:f>
+              <c:f>iterations!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2189,7 +2189,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'image-size'!$D$7:$D$19</c:f>
+              <c:f>iterations!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2294,11 +2294,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1455026960"/>
-        <c:axId val="1455034032"/>
+        <c:axId val="-34667824"/>
+        <c:axId val="-34666736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1455026960"/>
+        <c:axId val="-34667824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2402,7 +2402,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1455034032"/>
+        <c:crossAx val="-34666736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2410,7 +2410,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1455034032"/>
+        <c:axId val="-34666736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2518,7 +2518,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1455026960"/>
+        <c:crossAx val="-34667824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2696,7 +2696,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'image-size'!$D$22:$D$34</c:f>
+              <c:f>iterations!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2812,7 +2812,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'image-size'!$D$22:$D$34</c:f>
+              <c:f>iterations!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -2928,7 +2928,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'image-size'!$D$22:$D$34</c:f>
+              <c:f>iterations!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3044,7 +3044,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'image-size'!$D$22:$D$34</c:f>
+              <c:f>iterations!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3149,11 +3149,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1455025328"/>
-        <c:axId val="1455022608"/>
+        <c:axId val="-34660752"/>
+        <c:axId val="-34662384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1455025328"/>
+        <c:axId val="-34660752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3257,7 +3257,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1455022608"/>
+        <c:crossAx val="-34662384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3265,7 +3265,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1455022608"/>
+        <c:axId val="-34662384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3372,7 +3372,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1455025328"/>
+        <c:crossAx val="-34660752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3560,7 +3560,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'image-size'!$D$52:$D$64</c:f>
+              <c:f>iterations!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3676,7 +3676,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'image-size'!$D$52:$D$64</c:f>
+              <c:f>iterations!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3792,7 +3792,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'image-size'!$D$52:$D$64</c:f>
+              <c:f>iterations!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -3908,7 +3908,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'image-size'!$D$52:$D$64</c:f>
+              <c:f>iterations!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -4013,11 +4013,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1455027504"/>
-        <c:axId val="1455025872"/>
+        <c:axId val="-34665104"/>
+        <c:axId val="-34665648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1455027504"/>
+        <c:axId val="-34665104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4121,7 +4121,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1455025872"/>
+        <c:crossAx val="-34665648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4129,7 +4129,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1455025872"/>
+        <c:axId val="-34665648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4237,7 +4237,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1455027504"/>
+        <c:crossAx val="-34665104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4415,7 +4415,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'image-size'!$D$22:$D$34</c:f>
+              <c:f>'image-size'!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -4531,7 +4531,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'image-size'!$D$22:$D$34</c:f>
+              <c:f>'image-size'!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -4647,7 +4647,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'image-size'!$D$22:$D$34</c:f>
+              <c:f>'image-size'!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -4763,7 +4763,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'image-size'!$D$22:$D$34</c:f>
+              <c:f>'image-size'!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -4868,11 +4868,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1414994080"/>
-        <c:axId val="1255109920"/>
+        <c:axId val="-77687712"/>
+        <c:axId val="-77683904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1414994080"/>
+        <c:axId val="-77687712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4976,7 +4976,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1255109920"/>
+        <c:crossAx val="-77683904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4984,7 +4984,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1255109920"/>
+        <c:axId val="-77683904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5091,7 +5091,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1414994080"/>
+        <c:crossAx val="-77687712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5273,7 +5273,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'image-size'!$D$52:$D$64</c:f>
+              <c:f>'image-size'!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -5389,7 +5389,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'image-size'!$D$52:$D$64</c:f>
+              <c:f>'image-size'!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -5505,7 +5505,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'image-size'!$D$52:$D$64</c:f>
+              <c:f>'image-size'!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -5621,7 +5621,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'image-size'!$D$52:$D$64</c:f>
+              <c:f>'image-size'!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -5726,11 +5726,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1255113728"/>
-        <c:axId val="1415004960"/>
+        <c:axId val="-77698592"/>
+        <c:axId val="-101023392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1255113728"/>
+        <c:axId val="-77698592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5834,7 +5834,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1415004960"/>
+        <c:crossAx val="-101023392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5842,7 +5842,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1415004960"/>
+        <c:axId val="-101023392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5950,7 +5950,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1255113728"/>
+        <c:crossAx val="-77698592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6131,7 +6131,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'[1]image-size'!$D$7:$D$19</c:f>
+              <c:f>rectangle!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -6187,16 +6187,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0559838923537788</c:v>
+                  <c:v>1.9517168811103121</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.234816409693221</c:v>
+                  <c:v>3.9297092898519632</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.191363501922508</c:v>
+                  <c:v>5.9403656707341792</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.086476642476752</c:v>
+                  <c:v>7.8693375580677207</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>9.9208530805687207</c:v>
@@ -6247,7 +6247,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'[1]image-size'!$D$7:$D$19</c:f>
+              <c:f>rectangle!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -6363,7 +6363,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'[1]image-size'!$D$7:$D$19</c:f>
+              <c:f>rectangle!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -6479,7 +6479,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'[1]image-size'!$D$7:$D$19</c:f>
+              <c:f>rectangle!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -6584,11 +6584,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1455024240"/>
-        <c:axId val="1455033488"/>
+        <c:axId val="-101026656"/>
+        <c:axId val="-34661840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1455024240"/>
+        <c:axId val="-101026656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6692,7 +6692,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1455033488"/>
+        <c:crossAx val="-34661840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6700,7 +6700,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1455033488"/>
+        <c:axId val="-34661840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6808,7 +6808,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1455024240"/>
+        <c:crossAx val="-101026656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6991,7 +6991,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'[1]image-size'!$D$22:$D$34</c:f>
+              <c:f>rectangle!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -7047,16 +7047,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0279919461768894</c:v>
+                  <c:v>0.97585844055515603</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0587041024233053</c:v>
+                  <c:v>0.9824273224629908</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0318939169870847</c:v>
+                  <c:v>0.9900609451223632</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.010809580309594</c:v>
+                  <c:v>0.98366719475846509</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.99208530805687212</c:v>
@@ -7107,7 +7107,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'[1]image-size'!$D$22:$D$34</c:f>
+              <c:f>rectangle!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -7223,7 +7223,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'[1]image-size'!$D$22:$D$34</c:f>
+              <c:f>rectangle!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -7328,11 +7328,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1455023696"/>
-        <c:axId val="1455036752"/>
+        <c:axId val="-34664016"/>
+        <c:axId val="-34661296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1455023696"/>
+        <c:axId val="-34664016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7436,7 +7436,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1455036752"/>
+        <c:crossAx val="-34661296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7444,7 +7444,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1455036752"/>
+        <c:axId val="-34661296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7551,7 +7551,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1455023696"/>
+        <c:crossAx val="-34664016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7739,7 +7739,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'[1]image-size'!$D$52:$D$64</c:f>
+              <c:f>rectangle!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -7795,16 +7795,16 @@
                   <c:v>293062</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>285082</c:v>
+                  <c:v>300312</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>276812</c:v>
+                  <c:v>298304</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>284004</c:v>
+                  <c:v>296004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>289928</c:v>
+                  <c:v>297928</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>295400</c:v>
@@ -7855,7 +7855,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'[1]image-size'!$D$52:$D$64</c:f>
+              <c:f>rectangle!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -7971,7 +7971,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'[1]image-size'!$D$52:$D$64</c:f>
+              <c:f>rectangle!$D$7:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -8076,11 +8076,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1455037840"/>
-        <c:axId val="1455024784"/>
+        <c:axId val="-34663472"/>
+        <c:axId val="-34672720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1455037840"/>
+        <c:axId val="-34663472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8184,7 +8184,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1455024784"/>
+        <c:crossAx val="-34672720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8192,7 +8192,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1455024784"/>
+        <c:axId val="-34672720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8300,7 +8300,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1455037840"/>
+        <c:crossAx val="-34663472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8538,16 +8538,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0559838923537788</c:v>
+                  <c:v>1.9517168811103121</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.234816409693221</c:v>
+                  <c:v>3.9297092898519632</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.191363501922508</c:v>
+                  <c:v>5.9403656707341792</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.086476642476752</c:v>
+                  <c:v>7.8693375580677207</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>9.9208530805687207</c:v>
@@ -8935,11 +8935,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1455032400"/>
-        <c:axId val="1455031856"/>
+        <c:axId val="-34662928"/>
+        <c:axId val="-34667280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1455032400"/>
+        <c:axId val="-34662928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9043,7 +9043,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1455031856"/>
+        <c:crossAx val="-34667280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9051,7 +9051,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1455031856"/>
+        <c:axId val="-34667280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9159,7 +9159,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1455032400"/>
+        <c:crossAx val="-34662928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9393,16 +9393,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0279919461768894</c:v>
+                  <c:v>0.97585844055515603</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0587041024233053</c:v>
+                  <c:v>0.9824273224629908</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0318939169870847</c:v>
+                  <c:v>0.9900609451223632</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.010809580309594</c:v>
+                  <c:v>0.98366719475846509</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.99208530805687212</c:v>
@@ -9674,11 +9674,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1455037296"/>
-        <c:axId val="1455028592"/>
+        <c:axId val="-34666192"/>
+        <c:axId val="-34669456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1455037296"/>
+        <c:axId val="-34666192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9782,7 +9782,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1455028592"/>
+        <c:crossAx val="-34669456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9790,7 +9790,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1455028592"/>
+        <c:axId val="-34669456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9897,7 +9897,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1455037296"/>
+        <c:crossAx val="-34666192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10135,16 +10135,16 @@
                   <c:v>293062</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>285082</c:v>
+                  <c:v>300312</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>276812</c:v>
+                  <c:v>298304</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>284004</c:v>
+                  <c:v>296004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>289928</c:v>
+                  <c:v>297928</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>295400</c:v>
@@ -10416,11 +10416,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1455035664"/>
-        <c:axId val="1455029136"/>
+        <c:axId val="-34671088"/>
+        <c:axId val="-34664560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1455035664"/>
+        <c:axId val="-34671088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10524,7 +10524,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1455029136"/>
+        <c:crossAx val="-34664560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10532,7 +10532,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1455029136"/>
+        <c:axId val="-34664560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10640,7 +10640,7 @@
             <a:endParaRPr lang="bg-BG"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1455035664"/>
+        <c:crossAx val="-34671088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -18268,8 +18268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:M64"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AC37" sqref="AC37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19954,7 +19954,7 @@
         <v>24</v>
       </c>
       <c r="E49" s="1">
-        <v>17117</v>
+        <v>17137</v>
       </c>
       <c r="F49" s="1">
         <v>17256</v>
@@ -20568,8 +20568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:M62"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20586,6 +20586,10 @@
       <c r="B3" t="s">
         <v>22</v>
       </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -20699,32 +20703,32 @@
         <v>150418</v>
       </c>
       <c r="F8" s="1">
-        <v>142541</v>
+        <v>152541</v>
       </c>
       <c r="G8" s="1">
-        <v>146540</v>
+        <v>150540</v>
       </c>
       <c r="H8" s="1">
-        <v>145156</v>
+        <v>150156</v>
       </c>
       <c r="I8">
-        <v>142739</v>
+        <v>151739</v>
       </c>
       <c r="J8" s="7">
         <f t="shared" ref="J8:J19" si="1">MIN(E8:I8)</f>
-        <v>142541</v>
+        <v>150156</v>
       </c>
       <c r="K8" s="7">
         <f>$J$7/J8</f>
-        <v>2.0559838923537788</v>
+        <v>1.9517168811103121</v>
       </c>
       <c r="L8" s="7">
         <f t="shared" ref="L8:L19" si="2">K8/D8</f>
-        <v>1.0279919461768894</v>
+        <v>0.97585844055515603</v>
       </c>
       <c r="M8" s="7">
         <f t="shared" si="0"/>
-        <v>285082</v>
+        <v>300312</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -20736,35 +20740,35 @@
         <v>4</v>
       </c>
       <c r="E9" s="1">
-        <v>71646</v>
+        <v>75646</v>
       </c>
       <c r="F9" s="1">
-        <v>69948</v>
+        <v>75948</v>
       </c>
       <c r="G9" s="1">
-        <v>69203</v>
+        <v>76203</v>
       </c>
       <c r="H9" s="1">
-        <v>70556</v>
+        <v>74576</v>
       </c>
       <c r="I9">
-        <v>70065</v>
+        <v>75065</v>
       </c>
       <c r="J9" s="7">
         <f t="shared" si="1"/>
-        <v>69203</v>
+        <v>74576</v>
       </c>
       <c r="K9" s="7">
         <f t="shared" ref="K9:K19" si="3">$J$7/J9</f>
-        <v>4.234816409693221</v>
+        <v>3.9297092898519632</v>
       </c>
       <c r="L9" s="7">
         <f t="shared" si="2"/>
-        <v>1.0587041024233053</v>
+        <v>0.9824273224629908</v>
       </c>
       <c r="M9" s="7">
         <f t="shared" si="0"/>
-        <v>276812</v>
+        <v>298304</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -20776,35 +20780,35 @@
         <v>6</v>
       </c>
       <c r="E10" s="1">
-        <v>47334</v>
+        <v>49334</v>
       </c>
       <c r="F10" s="1">
-        <v>47356</v>
+        <v>50356</v>
       </c>
       <c r="G10" s="1">
-        <v>47756</v>
+        <v>49756</v>
       </c>
       <c r="H10" s="1">
-        <v>47611</v>
+        <v>49611</v>
       </c>
       <c r="I10">
-        <v>47612</v>
+        <v>50612</v>
       </c>
       <c r="J10" s="7">
         <f t="shared" si="1"/>
-        <v>47334</v>
+        <v>49334</v>
       </c>
       <c r="K10" s="7">
         <f t="shared" si="3"/>
-        <v>6.191363501922508</v>
+        <v>5.9403656707341792</v>
       </c>
       <c r="L10" s="7">
         <f t="shared" si="2"/>
-        <v>1.0318939169870847</v>
+        <v>0.9900609451223632</v>
       </c>
       <c r="M10" s="7">
         <f t="shared" si="0"/>
-        <v>284004</v>
+        <v>296004</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -20816,35 +20820,35 @@
         <v>8</v>
       </c>
       <c r="E11" s="1">
-        <v>36241</v>
+        <v>37241</v>
       </c>
       <c r="F11" s="1">
-        <v>36462</v>
+        <v>38462</v>
       </c>
       <c r="G11" s="1">
-        <v>36504</v>
+        <v>37504</v>
       </c>
       <c r="H11" s="1">
-        <v>36362</v>
+        <v>37362</v>
       </c>
       <c r="I11">
-        <v>36291</v>
+        <v>37291</v>
       </c>
       <c r="J11" s="7">
         <f t="shared" si="1"/>
-        <v>36241</v>
+        <v>37241</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" si="3"/>
-        <v>8.086476642476752</v>
+        <v>7.8693375580677207</v>
       </c>
       <c r="L11" s="7">
         <f t="shared" si="2"/>
-        <v>1.010809580309594</v>
+        <v>0.98366719475846509</v>
       </c>
       <c r="M11" s="7">
         <f t="shared" si="0"/>
-        <v>289928</v>
+        <v>297928</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -22484,8 +22488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:M64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>